<commit_message>
Opio modify char/bar 032123
</commit_message>
<xml_diff>
--- a/academycity/data/ms/datasets/excel/raw_data/RAW DATA (607)_TEST.xlsx
+++ b/academycity/data/ms/datasets/excel/raw_data/RAW DATA (607)_TEST.xlsx
@@ -1840,8 +1840,8 @@
   </sheetPr>
   <dimension ref="A1:UX5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22267" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>